<commit_message>
Updated sprint backlog and fixed database connection errors
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westga365-my.sharepoint.com/personal/ja00069_my_westga_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{B4D7B3C1-104E-4F4C-9F25-31954CDF18F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4310EDA9-1BE4-4C54-B2F0-2C5C9B8B41D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7C7CFF-4E98-45A0-9EB7-EBE42DFA6006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Related User Story</t>
   </si>
@@ -213,62 +213,62 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -371,7 +371,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -395,7 +395,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1448,24 +1448,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="34.7265625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1477,16 +1477,16 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11"/>
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1505,102 +1505,108 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="17">
         <v>0</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="17">
         <v>6.5</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>1</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="17">
+        <v>12.5</v>
+      </c>
+      <c r="F5" s="26">
+        <v>12.5</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>3</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>0</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="7">
         <v>4</v>
       </c>
@@ -1611,11 +1617,11 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="7">
         <v>4</v>
       </c>
@@ -1626,26 +1632,30 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1654,8 +1664,8 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="12"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1664,17 +1674,17 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21">
         <f>SUM(E3:E12)</f>
-        <v>6.5</v>
+        <v>21.5</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(F3:F12)</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="G13" s="2">
         <f>SUM(G3:G12)</f>
@@ -1702,6 +1712,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -1948,15 +1967,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1964,6 +1974,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1978,14 +1996,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added in my actual work hours
Edited the sprint backlog to add my actual work hours for the features assigned to me.
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA09A75-0FB7-449E-BF3A-6C44DE749D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B9F347-65E6-459F-B9C2-7355F49DC142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20085" yWindow="2175" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Related User Story</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Rahman</t>
+  </si>
+  <si>
+    <t>Jabesi/Ahmad/Rahman</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32.5</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -395,10 +401,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1154,8 +1160,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1448,20 +1454,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="51.453125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="34.7265625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1490,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26"/>
       <c r="B2" s="25"/>
       <c r="C2" s="3" t="s">
@@ -1505,7 +1511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1519,14 +1525,18 @@
         <v>25</v>
       </c>
       <c r="E3" s="17">
-        <v>6.5</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="F3" s="23">
+        <v>5</v>
+      </c>
+      <c r="G3" s="23">
+        <v>3</v>
+      </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
@@ -1551,7 +1561,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
@@ -1576,7 +1586,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
@@ -1586,14 +1596,16 @@
       <c r="C6" s="17">
         <v>3</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="17"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1612,7 +1624,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1620,14 +1632,18 @@
       <c r="C8" s="7">
         <v>4</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1635,14 +1651,18 @@
       <c r="C9" s="7">
         <v>4</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1663,7 +1683,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
@@ -1674,7 +1694,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1684,21 +1704,21 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="18"/>
       <c r="D13" s="20"/>
       <c r="E13" s="21">
         <f>SUM(E3:E12)</f>
-        <v>32.5</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(F3:F12)</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G13" s="2">
         <f>SUM(G3:G12)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2">
         <f>SUM(H3:H12)</f>
@@ -1722,15 +1742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -1977,6 +1988,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1984,14 +2004,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2006,6 +2018,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated sprint backlog for this iteration
Updated sprint backlog for this iteration
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B9F347-65E6-459F-B9C2-7355F49DC142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C4EDB9-D917-48D6-A02E-A5C9ABFAD8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Related User Story</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Task Description</t>
   </si>
   <si>
-    <t>Initial Estimate</t>
-  </si>
-  <si>
     <t>Week 1</t>
   </si>
   <si>
@@ -71,58 +68,248 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Ahmad</t>
-  </si>
-  <si>
-    <t>Implement login and logout functionality. Display full name and username of logged-in nurses on all views.</t>
-  </si>
-  <si>
-    <t>Develop the patient registration form.</t>
-  </si>
-  <si>
-    <t>Implement the edit patient functionality. Patient information should be automatically loaded for updates.</t>
-  </si>
-  <si>
-    <t>Admin functionality to add nurses to the system.</t>
-  </si>
-  <si>
-    <t>Create the database on the departmental MySQL server for the project.</t>
-  </si>
-  <si>
-    <t>Project set up: follow practice exercise 11 for setting up a good structure, using Data Access Layer (DAL) in MVC/MVVM.</t>
-  </si>
-  <si>
-    <t>SQL Injection Mitigation: Use parameterized queries in C# or prepared statements in Java.</t>
-  </si>
-  <si>
-    <t>1. Design login and logout pages (UI) 2. Create database access for nurse login/logout. 3. Display nurse's full name and username on all views.</t>
-  </si>
-  <si>
-    <t>1. Design the patient registration UI. 2. Implement dropdown boxes for gender and state. 3. Perform field validation (zip code, phone number, etc.). 4. Create database access for patient registration.</t>
-  </si>
-  <si>
-    <t>1. Design the edit patient UI. 2. Implement auto-loading of patient information. 3. Create database access for editing patient information.</t>
-  </si>
-  <si>
-    <t>1. Design the nurse addition UI for admins. 2. Implement dropdown for roles (nurse/admin). 3. Create database access for adding nurses.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Email Edwin for database creation. 2. Write SQL statements to create tables. 3. </t>
-  </si>
-  <si>
-    <t>Revise the database design</t>
-  </si>
-  <si>
-    <t>Jabesi</t>
-  </si>
-  <si>
-    <t>Rahman</t>
-  </si>
-  <si>
-    <t>Jabesi/Ahmad/Rahman</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>Create an appointment</t>
+  </si>
+  <si>
+    <t>Enter routine checkup information</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Design Routine Checks UI </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add functionality to enter routine checks information and store it in the database (keep in mind systolic, diastolic blood pressure and pulse are integer values, weight (lb), height (in) is a decimal value)</t>
+    </r>
+  </si>
+  <si>
+    <t>Search for patient to show his/her appointment information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search for a patient by criteria </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add Search UI elements into the Manage_Patients form </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to search by date of birth, name (last and first), or both (note that the search should be done on the DB server side instead of the client side )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Design Search UI. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add functionality to search for patients and display their appointment information (same search criteria as above)</t>
+    </r>
+  </si>
+  <si>
+    <t>Edit Appointment if time has not passed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Design edit appointment UI. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to edit an appointment only if the time hasn't passed and save those changes to the database</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Design create appointment UI </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Add functionality to create appointments and save them in the database(Double booking isn't allowed and appointments are 20 minutes long)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmad </t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Estimate</t>
   </si>
 </sst>
 </file>
@@ -202,14 +389,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -234,9 +418,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -264,17 +445,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,9 +563,6 @@
               <c:f>Sheet1!$E$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>34</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -401,10 +585,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1455,276 +1639,226 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="19" customWidth="1"/>
-    <col min="4" max="4" width="34.7265625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="13">
         <v>7</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="F3" s="21">
+        <v>7</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="3" t="s">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="17">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16">
+        <f>SUM(F3:F12)</f>
+        <v>7</v>
+      </c>
+      <c r="G13" s="16">
+        <f>SUM(G3:G12)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="17">
-        <v>8</v>
-      </c>
-      <c r="F3" s="23">
-        <v>5</v>
-      </c>
-      <c r="G3" s="23">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="17">
-        <v>1</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="17">
-        <v>12</v>
-      </c>
-      <c r="F4" s="23">
-        <v>12</v>
-      </c>
-      <c r="G4" s="23">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="17">
-        <v>2</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="17">
-        <v>12</v>
-      </c>
-      <c r="F5" s="23">
-        <v>12</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="17">
-        <v>3</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="17">
-        <v>0</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="7">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7">
-        <v>2</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="10"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21">
-        <f>SUM(E3:E12)</f>
-        <v>34</v>
-      </c>
-      <c r="F13" s="2">
-        <f>SUM(F3:F12)</f>
-        <v>29</v>
-      </c>
-      <c r="G13" s="2">
-        <f>SUM(G3:G12)</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="H13" s="16">
         <f>SUM(H3:H12)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="16">
         <f>SUM(I3:I12)</f>
         <v>0</v>
       </c>
@@ -1742,6 +1876,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -1988,15 +2131,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2004,6 +2138,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2018,14 +2160,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated time remaining in sprint
Updated time remaining in sprint
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 1 (Itteration 2)  Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Documents\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84227817-3949-420B-80D4-C580E4DB6422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F303B3D4-5388-47A1-A5ED-BBE3A48F0088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="1545" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1723,7 +1723,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1801,9 @@
       <c r="F3" s="19">
         <v>7</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
@@ -1986,6 +1988,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2232,15 +2243,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2248,6 +2250,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2262,14 +2272,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>